<commit_message>
Add some more spreadsheets
</commit_message>
<xml_diff>
--- a/results/roundabout_full.txt_50_yaw.xlsx
+++ b/results/roundabout_full.txt_50_yaw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artyom\Documents\Projects\autonomous_vehicles1\path-planning-simulation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41B62837-BA3D-4DB7-A4EE-60BD3441C760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D78E2EF-BEC0-44EA-B7D3-9BC616A3A1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roundabout_full.txt_50_yaw" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,6 +578,4008 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Steering angle at 50 km/h,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> roundabout course</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pure Pursuit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$A$2:$A$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>11.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$B$2:$B$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-9.5229099808879E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-2.5608464064073501E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-6.1327120166210003E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.106684761074295</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.15873747704166999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.215284745510812</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.272861074560658</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.30634443274323903</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.311018353949511</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.30012020539193401</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.268460575853261</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.237576142683221</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.18087946118398601</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.136241108868313</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-6.1779964872737098E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.8161666509622601E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.12730053749321099</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.208925623998652</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.33960114089827997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.43449733256443801</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.55984318278647804</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.63212977269127801</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.66110381634117998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.67086028668643005</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.67050838405818503</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.66367665758338901</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.65086727441848202</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.63954261370114796</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.63304541955364702</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.62810746223311498</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.62745290791508701</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.63053621805223503</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.63690103772204898</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.64588197703599604</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.65691058917733502</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.66949988615621403</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.683229550606401</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.69773309328396804</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.71731068164180201</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.73188594199211998</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.75065455639682699</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.76429831800254899</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.77673176176485403</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.77201878600235596</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.75894128861375598</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.73834252072653705</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71103047404122899</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.67756198388739397</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.63815386269518803</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.59266966690206901</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.51591190905588902</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.46683265212060598</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.38775084152536898</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.31023706822656899</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.23438641117808501</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.16687002017666699</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.10630412332073701</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.3405984008911098E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3600145221997303E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-2.8026491114663599E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-5.78822031659815E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-8.1732955802747503E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-9.9659188391472697E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.11358877608611601</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.123055656347189</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.12919175697815399</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.132466724815131</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.133316118390743</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.13213816499723599</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-0.12937805746821199</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.12521302319842301</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.119975967235482</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.11392311395802</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.10747712453694</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.10041133415716</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-9.3112220952604297E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-8.5944199734371299E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-7.8545812620640698E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-7.1279927803187496E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-6.4228455311372404E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-5.7658341354730497E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-5.11685844840052E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-4.5048981223324097E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-3.9324685892004302E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-3.4169311920677299E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-2.92309634922172E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-2.6713292533866801E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-2.64663974417906E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-2.6166900881553198E-2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-2.5796005374370101E-2</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-2.53247457542807E-2</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-2.4706039475329001E-2</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-2.3857895846568E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A606-4C18-AE27-F83F7022F5C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stanley</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$A$2:$A$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>11.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$C$2:$C$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-8.4860103735007894E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.18138858953787099</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.334406118927701</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.37241574533232202</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.49558343896868001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.58658045747126697</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.65011246907201503</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.524605045261198</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.26021651025665299</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-5.5089774456507298E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.3219613836189098E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.22158429687343201</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.280997034217639</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.411343680597406</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.42754606412000301</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.549304710954165</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.63357300843035902</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.68925437001172396</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.68713551894262503</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.54238760504099803</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.43978938056189398</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.46596995168285898</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.51870364712040895</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.61030349186211696</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.73887013824888803</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.73990957615608499</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.46181546464136197</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.12106683300101399</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-6.1118780691396202E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-9.56809366319194E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-0.11688040805161901</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-0.13033690804561801</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-0.136037737262408</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-0.13635812004683101</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.13305142802453801</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.12738909601619799</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.120282451362646</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.11119201428346399</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.103498061234752</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-9.55999081894673E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-8.7764714716102699E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-8.0172271085507799E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-7.2938981829858598E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-6.6135376052424505E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-5.9798962453398198E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-5.3943715198650502E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-4.81045955980016E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-4.3411157848015101E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-3.90890894420797E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-3.5133336135904601E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-3.1530661419063299E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-2.7997169180097901E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-2.5168012339699199E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-2.2587648307311099E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-2.0244811533022801E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-1.8125365769680001E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-1.60622488054749E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-1.44137465111479E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-1.29168077058592E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-1.15626169587239E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-1.02448203537975E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-9.1916771320978592E-3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-8.2355867570114098E-3</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-7.3708791655095699E-3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-5.7928117388928203E-3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-3.90266474088731E-3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-2.7376769758653201E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A606-4C18-AE27-F83F7022F5C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stanley with lookahead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$A$2:$A$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>11.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$D$2:$D$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-8.4860103735007894E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.24607051907741301</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.290618218904587</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.412804663185451</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.40947257014744998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.51400541553539303</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.68966966387810502</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.38424903144492301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.15009205457590999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.6780655260214199E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.132452794880314</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.256934941710803</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.28535496144459399</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.39255561976444697</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.387646763708415</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.486660710084027</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.55674289688283496</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.60609700054562199</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.751812907470641</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.70642655532116505</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.60632379570349204</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.457667910763634</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.58322260648380797</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.68325740721225403</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.45214627080432601</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.25046109396136701</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.103205769601744</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.0009064145118301E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-4.3113799154771898E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-7.2462866609242199E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-8.7035291929536504E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-9.20328276792267E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-9.2460792074816694E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-9.0059912837096898E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-8.4906132111500804E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-7.9473117031265306E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-7.4928852855548705E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-6.9116369246950499E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-6.3691118135418001E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-5.8643418242559399E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-5.3959096818416298E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-4.9621149369814203E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-4.5610925293162498E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-4.1908976680650398E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-3.8495664201574402E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-3.5351585615284099E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-3.2062134965748001E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-2.9600313012756101E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-2.7277527109921099E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-2.5104140855222799E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-2.30823378948916E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-2.1209248869498099E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1.92413156996263E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-1.7766264901642799E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-1.6372531009294401E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-1.50674870392068E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-1.3853095552475299E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-1.25725429846809E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-1.16117509470709E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-8.3399404995503305E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-5.1957202455225303E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-3.38127900161596E-3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-2.294407577804E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A606-4C18-AE27-F83F7022F5C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid Stanley and Pure Pursuit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$A$2:$A$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>11.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'roundabout_full.txt_50_yaw'!$E$2:$E$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="118"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-8.4860103735007894E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.18138858953787099</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.334406118927701</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.37241574533232202</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.49558343896868001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.58658045747126697</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.65011246907201503</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.524605045261198</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.26021651025665299</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-5.5089774456507298E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.3219613836189098E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.22158429687343201</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.280997034217639</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.411343680597406</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.41137605963358698</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.55652481553787303</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.63760099931446701</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.69121539180712999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.49163897916042498</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.49544377899273401</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.50615160005133597</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.51868179643994194</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.54117950088467603</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.56280237133269995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58623230442156704</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.61876910436890398</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.64294937463157098</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.67489764668850505</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.70499510553607803</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.73299271931434296</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.75871024794651398</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.78539816339744795</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.77760397412021098</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.75633974468917198</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.74337268019954905</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71140440533383698</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.67369075464480699</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.63015849795345802</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.58037485614905204</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.51003112948769702</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.43496584590807402</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.35770761986733401</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.28310400082958798</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.21310076470627601</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.149230716730202</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.2490377098225204E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.3334894615571898E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.9154052539355898E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-3.0879101852888901E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-5.84681461263835E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-8.0395411780301199E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-9.6780486589366305E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.23208177383798401</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.20296086439491301</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.17686366940793</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.15660381450351099</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.13761006775874601</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.121445952627634</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-0.10751860699441999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-9.5404590548208296E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-8.4792569555130301E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-7.5447063140104895E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-6.6563457965439304E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-5.9534714770086303E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-5.3225406960122797E-2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-4.7565175043851E-2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-4.2490706418344397E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-3.7944655051569999E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-3.3560077164610201E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-3.0068577109376899E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-2.6913175443940202E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-2.4069040213303101E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-2.1310771854597399E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-1.91091981377438E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-1.7113990187942799E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-1.53118649580666E-2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-1.36885563944772E-2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-1.21157823558273E-2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-1.0860715036559001E-2</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>8.3056923242255092E-3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>8.0256090487578497E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A606-4C18-AE27-F83F7022F5C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="884403968"/>
+        <c:axId val="884405216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="884403968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="884405216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="884405216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Steering angle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="884403968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF42127C-9DD2-46A2-85B6-D4B81CB47BEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -874,11 +4876,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="L111" sqref="L111"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection sqref="A1:E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2869,5 +6871,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>